<commit_message>
Added to the team contribution log
I added my highlights contribution to the team contribution log.
</commit_message>
<xml_diff>
--- a/Team Contribution Log.xlsx
+++ b/Team Contribution Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\back up of school files\Software Design &amp; Development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atm15_000\Documents\GitHub\SDDGroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Sprint #</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>The Scrum master collects and compiles this log by Sprint</t>
+  </si>
+  <si>
+    <t>Michael McGregor</t>
+  </si>
+  <si>
+    <t>Covered the project highlights for the propsal</t>
   </si>
 </sst>
 </file>
@@ -458,12 +464,13 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
     <col min="4" max="4" width="77.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -489,9 +496,15 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>

</xml_diff>

<commit_message>
Created project file for use for the group, created model, view, controller folders and moved the java files into the project as a starter point.
</commit_message>
<xml_diff>
--- a/Team Contribution Log.xlsx
+++ b/Team Contribution Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atm15_000\Documents\GitHub\SDDGroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\back up of school files\Software Design &amp; Development\SDDGroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Sprint #</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Covered the project highlights for the propsal</t>
+  </si>
+  <si>
+    <t>Will McLain</t>
+  </si>
+  <si>
+    <t>Covered the working agreement for the propsal</t>
   </si>
 </sst>
 </file>
@@ -507,9 +513,15 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>

</xml_diff>

<commit_message>
updated sprint backlog, and updated contribution log for items I am aware of
</commit_message>
<xml_diff>
--- a/Team Contribution Log.xlsx
+++ b/Team Contribution Log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Sprint #</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Edited video for sprint 1</t>
+  </si>
+  <si>
+    <t>Edited video for sprint 2</t>
   </si>
 </sst>
 </file>
@@ -488,7 +491,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -597,9 +600,15 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>

</xml_diff>

<commit_message>
updates for contribution log
</commit_message>
<xml_diff>
--- a/Team Contribution Log.xlsx
+++ b/Team Contribution Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atm15_000\Documents\GitHub\SDDGroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\back up of school files\Software Design &amp; Development\SDDGroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Sprint #</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Integration debugging</t>
+  </si>
+  <si>
+    <t>Helped Ryan with the enemy collisions and debugging</t>
+  </si>
+  <si>
+    <t>Edited video for sprint 3</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -636,14 +642,26 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>

</xml_diff>